<commit_message>
set datetime format in excel example file to whole column
</commit_message>
<xml_diff>
--- a/src/main/resources/static/investbook-format-example.xlsx
+++ b/src/main/resources/static/investbook-format-example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Витек\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\investbook\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -193,13 +193,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,6 +215,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -502,136 +501,136 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="18" style="9" customWidth="1"/>
+    <col min="9" max="9" width="21" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C2" s="2">
         <v>44207.416666666664</v>
       </c>
       <c r="F2">
         <v>10000</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C3" s="2">
         <v>44207.458333333336</v>
       </c>
       <c r="F3">
         <v>100</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C4" s="2">
         <v>44209.427083333336</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>10</v>
       </c>
       <c r="F4">
         <v>250</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="I4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="5">
         <v>1.5</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C5" s="2">
         <v>44208.430567129632</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>1</v>
       </c>
       <c r="F5">
@@ -640,276 +639,276 @@
       <c r="G5">
         <v>12.01</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="7">
+      <c r="I5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5">
         <v>0.6</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C6" s="3">
         <v>44328.416666666664</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>10</v>
       </c>
       <c r="F6">
         <v>187</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="7">
+      <c r="I6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="5">
         <v>24</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C7" s="3">
         <v>44496.416666666664</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>10</v>
       </c>
       <c r="F7">
         <v>161</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="I7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="5">
         <v>20</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C8" s="3">
         <v>44081.416666666664</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>2</v>
       </c>
       <c r="F8">
         <v>600</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C9" s="3">
         <v>44095.416666666664</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>2</v>
       </c>
       <c r="F9">
         <v>1400</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C10" s="3">
         <v>44212.5</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <v>130</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C11" s="3">
         <v>44331.5</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <v>52000</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C12" s="3">
         <v>44331.416666666664</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>30</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C13" s="3">
         <v>44211.5</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>300</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C14" s="3">
         <v>44212.5</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>100</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C15" s="3">
         <v>44074.416666666664</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C16" s="3">
         <v>44074.416666666664</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="2">
         <v>44576.583333333336</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>1</v>
       </c>
       <c r="F17">
         <v>38600</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C18" s="2">
         <v>44574.520833333336</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="10">
         <v>1</v>
       </c>
       <c r="F18">
@@ -918,76 +917,76 @@
       <c r="H18">
         <v>60120</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="7">
+      <c r="I18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="5">
         <v>3.05</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C19" s="2">
         <v>44574.791666666664</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="10">
         <v>1</v>
       </c>
       <c r="F19">
         <v>75</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C20" s="2">
         <v>44575.791666666664</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="10">
         <v>1</v>
       </c>
       <c r="F20">
         <v>-20</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C21" s="2">
         <v>44309.583333333336</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="10">
         <v>1</v>
       </c>
       <c r="F21">
@@ -996,47 +995,47 @@
       <c r="H21">
         <v>2600</v>
       </c>
-      <c r="I21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="7">
+      <c r="I21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="5">
         <v>2.95</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B22" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C22" s="2">
         <v>44211.791666666664</v>
       </c>
       <c r="F22">
         <v>1500</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="9">
-        <v>111222</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C23" s="2">
         <v>44211.791666666664</v>
       </c>
       <c r="F23">
         <v>20000</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
expect security cash flow for one security (except derivative profit)
</commit_message>
<xml_diff>
--- a/src/main/resources/static/investbook-format-example.xlsx
+++ b/src/main/resources/static/investbook-format-example.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
   </bookViews>
   <sheets>
-    <sheet name="Данные" sheetId="1" r:id="rId1"/>
-    <sheet name="Спавочник Событий" sheetId="2" r:id="rId2"/>
+    <sheet name="investbook-format-example" sheetId="1" r:id="rId1"/>
+    <sheet name="Список допустимых событий" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>Ввод денежных средств</t>
   </si>
@@ -69,9 +69,6 @@
     <t>BR-3.22</t>
   </si>
   <si>
-    <t>Комиссия / Налог</t>
-  </si>
-  <si>
     <t>Валюта комиссии / налога</t>
   </si>
   <si>
@@ -141,10 +138,22 @@
     <t>Стоимость одного срочного контракта в валюте на момент сделки (опционально)</t>
   </si>
   <si>
-    <t>Цена одной ЦБ / Выплата (на все ЦБ до налога)</t>
-  </si>
-  <si>
     <t>НКД одной облигации на момент сделки</t>
+  </si>
+  <si>
+    <t>USDRUB_TOM</t>
+  </si>
+  <si>
+    <t>Цена одной ЦБ /
+Котировка контракта /
+Выплата (на одну ЦБ до налога) /
+Вариационная маржа (на все контракты) /
+Цена единицы товара /
+Перевод или остаток денежных средств</t>
+  </si>
+  <si>
+    <t>Комиссия / Налог
+(на событие вцелом, на все бумаги)</t>
   </si>
 </sst>
 </file>
@@ -498,60 +507,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="8" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" customWidth="1"/>
     <col min="9" max="9" width="21" style="7" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="5" customWidth="1"/>
     <col min="11" max="11" width="18" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -628,10 +635,10 @@
         <v>44208.430567129632</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>998.5</v>
@@ -666,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="F6">
-        <v>187</v>
+        <v>18.7</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>9</v>
@@ -689,13 +696,13 @@
         <v>44496.416666666664</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="10">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>161</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>9</v>
@@ -709,7 +716,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7">
         <v>111222</v>
@@ -718,13 +725,13 @@
         <v>44081.416666666664</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>9</v>
@@ -732,7 +739,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7">
         <v>111222</v>
@@ -741,13 +748,13 @@
         <v>44095.416666666664</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="10">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>1400</v>
+        <v>700</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>9</v>
@@ -772,7 +779,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="7">
         <v>111222</v>
@@ -789,7 +796,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="7">
         <v>111222</v>
@@ -806,7 +813,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7">
         <v>111222</v>
@@ -823,7 +830,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7">
         <v>111222</v>
@@ -849,7 +856,7 @@
         <v>44074.416666666664</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -866,7 +873,7 @@
         <v>44074.416666666664</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="10">
         <v>4</v>
@@ -877,16 +884,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2">
         <v>44576.583333333336</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>38600</v>
@@ -909,7 +916,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>80</v>
@@ -941,10 +948,10 @@
         <v>13</v>
       </c>
       <c r="E19" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>9</v>
@@ -964,10 +971,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>-20</v>
+        <v>-40</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>9</v>
@@ -984,10 +991,10 @@
         <v>44309.583333333336</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>2600</v>
@@ -1007,18 +1014,30 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B22" s="7">
         <v>111222</v>
       </c>
       <c r="C22" s="2">
-        <v>44211.791666666664</v>
+        <v>44309.583333333336</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2000</v>
       </c>
       <c r="F22">
-        <v>1500</v>
+        <v>70</v>
       </c>
       <c r="I22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="5">
+        <v>42</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1033,9 +1052,26 @@
         <v>44211.791666666664</v>
       </c>
       <c r="F23">
+        <v>1500</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="7">
+        <v>111222</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44211.791666666664</v>
+      </c>
+      <c r="F24">
         <v>20000</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1047,9 +1083,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Спавочник Событий'!$A$1:$A$18</xm:f>
+            <xm:f>'Список допустимых событий'!$A$1:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A10340</xm:sqref>
+          <xm:sqref>A2:A10341</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1061,7 +1097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1100,12 +1138,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1125,22 +1163,22 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -1150,12 +1188,12 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>